<commit_message>
Country data - population density and Urban Popluation%
</commit_message>
<xml_diff>
--- a/Inventory of Keyboard Combinations.xlsx
+++ b/Inventory of Keyboard Combinations.xlsx
@@ -1057,7 +1057,7 @@
     <col min="4" max="50" width="5.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:50" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:50" ht="21" x14ac:dyDescent="0.25">
       <c r="B1" s="8" t="s">
         <v>89</v>
       </c>
@@ -15087,7 +15087,7 @@
     <col min="4" max="68" width="5.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:68" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:68" ht="21" x14ac:dyDescent="0.25">
       <c r="B1" s="8" t="s">
         <v>89</v>
       </c>

</xml_diff>